<commit_message>
feat: Nova tela (funil)
</commit_message>
<xml_diff>
--- a/funil_consolidado.xlsx
+++ b/funil_consolidado.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,287 +456,287 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>APOGEU SANTO ANTÔNIO II</t>
+          <t>COLEGIO E CURSO MATRIZ EDUCACAO BANGU</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1582</v>
+        <v>1877</v>
       </c>
       <c r="C2" t="n">
-        <v>950</v>
+        <v>1219</v>
       </c>
       <c r="D2" t="n">
-        <v>837</v>
+        <v>1069</v>
       </c>
       <c r="E2" t="n">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="F2" t="n">
-        <v>423</v>
+        <v>877</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>COLEGIO E CURSO MATRIZ EDUCACAO BANGU</t>
+          <t>COLEGIO E CURSO MATRIZ EDUCACAO CAMPO GRANDE</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1861</v>
+        <v>1889</v>
       </c>
       <c r="C3" t="n">
-        <v>1202</v>
+        <v>1564</v>
       </c>
       <c r="D3" t="n">
-        <v>1056</v>
+        <v>1462</v>
       </c>
       <c r="E3" t="n">
-        <v>379</v>
+        <v>555</v>
       </c>
       <c r="F3" t="n">
-        <v>405</v>
+        <v>845</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>COLEGIO E CURSO MATRIZ EDUCACAO CAMPO GRANDE</t>
+          <t>COLÉGIO LEONARDO DA VINCI - ALFA</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1863</v>
+        <v>1220</v>
       </c>
       <c r="C4" t="n">
-        <v>1540</v>
+        <v>717</v>
       </c>
       <c r="D4" t="n">
-        <v>1438</v>
+        <v>519</v>
       </c>
       <c r="E4" t="n">
-        <v>555</v>
+        <v>371</v>
       </c>
       <c r="F4" t="n">
-        <v>305</v>
+        <v>834</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>COLÉGIO E CURSO CUBO BARRA GOLF</t>
+          <t>APOGEU BENFICA</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2288</v>
+        <v>1142</v>
       </c>
       <c r="C5" t="n">
-        <v>956</v>
+        <v>873</v>
       </c>
       <c r="D5" t="n">
-        <v>673</v>
+        <v>800</v>
       </c>
       <c r="E5" t="n">
-        <v>460</v>
+        <v>295</v>
       </c>
       <c r="F5" t="n">
-        <v>303</v>
+        <v>790</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>APOGEU SANTO ANTÔNIO I</t>
+          <t>APOGEU SANTO ANTÔNIO II</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1924</v>
+        <v>1608</v>
       </c>
       <c r="C6" t="n">
-        <v>1569</v>
+        <v>973</v>
       </c>
       <c r="D6" t="n">
-        <v>1466</v>
+        <v>858</v>
       </c>
       <c r="E6" t="n">
-        <v>518</v>
+        <v>377</v>
       </c>
       <c r="F6" t="n">
-        <v>293</v>
+        <v>751</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>COLÉGIO QI VALQUEIRE</t>
+          <t>COLÉGIO LEONARDO DA VINCI - BETA</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2675</v>
+        <v>715</v>
       </c>
       <c r="C7" t="n">
-        <v>767</v>
+        <v>438</v>
       </c>
       <c r="D7" t="n">
-        <v>615</v>
+        <v>327</v>
       </c>
       <c r="E7" t="n">
-        <v>562</v>
+        <v>238</v>
       </c>
       <c r="F7" t="n">
-        <v>278</v>
+        <v>749</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>COLEGIO E CURSO MATRIZ EDUCACAO RETIRO DOS ARTISTAS</t>
+          <t>APOGEU GLOBAL SCHOOL FERREIRA GUIMARÃES</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>952</v>
+        <v>1010</v>
       </c>
       <c r="C8" t="n">
-        <v>711</v>
+        <v>903</v>
       </c>
       <c r="D8" t="n">
-        <v>645</v>
+        <v>514</v>
       </c>
       <c r="E8" t="n">
-        <v>355</v>
+        <v>374</v>
       </c>
       <c r="F8" t="n">
-        <v>277</v>
+        <v>733</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>APOGEU GLOBAL SCHOOL FERREIRA GUIMARÃES</t>
+          <t>APOGEU SANTO ANTÔNIO I</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1006</v>
+        <v>1943</v>
       </c>
       <c r="C9" t="n">
-        <v>902</v>
+        <v>1585</v>
       </c>
       <c r="D9" t="n">
-        <v>513</v>
+        <v>1481</v>
       </c>
       <c r="E9" t="n">
-        <v>373</v>
+        <v>518</v>
       </c>
       <c r="F9" t="n">
-        <v>274</v>
+        <v>707</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>COLEGIO E CURSO MATRIZ EDUCACAO TAQUARA</t>
+          <t>COLEGIO E CURSO MATRIZ EDUCACAO ROCHA MIRANDA</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1179</v>
+        <v>765</v>
       </c>
       <c r="C10" t="n">
-        <v>867</v>
+        <v>580</v>
       </c>
       <c r="D10" t="n">
-        <v>770</v>
+        <v>526</v>
       </c>
       <c r="E10" t="n">
-        <v>284</v>
+        <v>175</v>
       </c>
       <c r="F10" t="n">
-        <v>245</v>
+        <v>700</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ESCOLA SAP</t>
+          <t>APOGEU GLOBAL SCHOOL CIDADE ALTA</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1834</v>
+        <v>388</v>
       </c>
       <c r="C11" t="n">
-        <v>374</v>
+        <v>189</v>
       </c>
       <c r="D11" t="n">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="E11" t="n">
-        <v>131</v>
+        <v>69</v>
       </c>
       <c r="F11" t="n">
-        <v>226</v>
+        <v>673</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>COLEGIO E CURSO MATRIZ EDUCACAO MADUREIRA</t>
+          <t>COLEGIO E CURSO MATRIZ EDUCACAO TAQUARA</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>963</v>
+        <v>1196</v>
       </c>
       <c r="C12" t="n">
-        <v>726</v>
+        <v>883</v>
       </c>
       <c r="D12" t="n">
-        <v>662</v>
+        <v>785</v>
       </c>
       <c r="E12" t="n">
-        <v>217</v>
+        <v>284</v>
       </c>
       <c r="F12" t="n">
-        <v>225</v>
+        <v>618</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>COLEGIO E CURSO MATRIZ EDUCACAO ROCHA MIRANDA</t>
+          <t>ESCOLA SA PEREIRA (R. DA MATRIZ)</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>757</v>
+        <v>1090</v>
       </c>
       <c r="C13" t="n">
-        <v>577</v>
+        <v>453</v>
       </c>
       <c r="D13" t="n">
-        <v>523</v>
+        <v>268</v>
       </c>
       <c r="E13" t="n">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="F13" t="n">
-        <v>216</v>
+        <v>593</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>COLÉGIO QI RIO 2</t>
+          <t>ESCOLA SAP</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1152</v>
+        <v>1838</v>
       </c>
       <c r="C14" t="n">
-        <v>407</v>
+        <v>375</v>
       </c>
       <c r="D14" t="n">
-        <v>319</v>
+        <v>200</v>
       </c>
       <c r="E14" t="n">
-        <v>271</v>
+        <v>132</v>
       </c>
       <c r="F14" t="n">
-        <v>197</v>
+        <v>566</v>
       </c>
     </row>
     <row r="15">
@@ -746,173 +746,173 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1073</v>
+        <v>1079</v>
       </c>
       <c r="C15" t="n">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D15" t="n">
         <v>232</v>
       </c>
       <c r="E15" t="n">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F15" t="n">
-        <v>155</v>
+        <v>566</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>COLÉGIO LEONARDO DA VINCI - ALFA</t>
+          <t>COLÉGIO QI RIO 2</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1208</v>
+        <v>1171</v>
       </c>
       <c r="C16" t="n">
-        <v>714</v>
+        <v>415</v>
       </c>
       <c r="D16" t="n">
-        <v>517</v>
+        <v>323</v>
       </c>
       <c r="E16" t="n">
-        <v>371</v>
+        <v>279</v>
       </c>
       <c r="F16" t="n">
-        <v>153</v>
+        <v>558</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>APOGEU BENFICA</t>
+          <t>COLEGIO SARAH DAWSEY - JUIZ DE FORA</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1126</v>
+        <v>1152</v>
       </c>
       <c r="C17" t="n">
-        <v>855</v>
+        <v>447</v>
       </c>
       <c r="D17" t="n">
-        <v>785</v>
+        <v>284</v>
       </c>
       <c r="E17" t="n">
-        <v>295</v>
+        <v>203</v>
       </c>
       <c r="F17" t="n">
-        <v>152</v>
+        <v>557</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>COLEGIO E CURSO MATRIZ EDUCACAO DUQUE DE CAXIAS</t>
+          <t>COLÉGIO E CURSO CUBO BARRA GOLF</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>898</v>
+        <v>2289</v>
       </c>
       <c r="C18" t="n">
-        <v>656</v>
+        <v>959</v>
       </c>
       <c r="D18" t="n">
-        <v>600</v>
+        <v>675</v>
       </c>
       <c r="E18" t="n">
-        <v>287</v>
+        <v>464</v>
       </c>
       <c r="F18" t="n">
-        <v>138</v>
+        <v>536</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>COLEGIO E CURSO MATRIZ EDUCACAO SÃO JOÃO DE MERITI</t>
+          <t>COLEGIO E CURSO MATRIZ EDUCACAO RETIRO DOS ARTISTAS</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>968</v>
+        <v>960</v>
       </c>
       <c r="C19" t="n">
-        <v>607</v>
+        <v>716</v>
       </c>
       <c r="D19" t="n">
-        <v>540</v>
+        <v>646</v>
       </c>
       <c r="E19" t="n">
-        <v>152</v>
+        <v>354</v>
       </c>
       <c r="F19" t="n">
-        <v>134</v>
+        <v>524</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>COLÉGIO LEONARDO DA VINCI - BETA</t>
+          <t>COLÉGIO QI TIJUCA</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>708</v>
+        <v>1042</v>
       </c>
       <c r="C20" t="n">
-        <v>437</v>
+        <v>224</v>
       </c>
       <c r="D20" t="n">
-        <v>326</v>
+        <v>169</v>
       </c>
       <c r="E20" t="n">
-        <v>236</v>
+        <v>142</v>
       </c>
       <c r="F20" t="n">
-        <v>133</v>
+        <v>503</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>APOGEU GLOBAL SCHOOL CIDADE ALTA</t>
+          <t>COLÉGIO AMERICANO</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>386</v>
+        <v>481</v>
       </c>
       <c r="C21" t="n">
-        <v>187</v>
+        <v>290</v>
       </c>
       <c r="D21" t="n">
-        <v>119</v>
+        <v>224</v>
       </c>
       <c r="E21" t="n">
-        <v>67</v>
+        <v>164</v>
       </c>
       <c r="F21" t="n">
-        <v>131</v>
+        <v>481</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>COLÉGIO QI TIJUCA</t>
+          <t>COLEGIO E CURSO MATRIZ EDUCACAO MADUREIRA</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1032</v>
+        <v>979</v>
       </c>
       <c r="C22" t="n">
+        <v>739</v>
+      </c>
+      <c r="D22" t="n">
+        <v>676</v>
+      </c>
+      <c r="E22" t="n">
         <v>217</v>
       </c>
-      <c r="D22" t="n">
-        <v>161</v>
-      </c>
-      <c r="E22" t="n">
-        <v>138</v>
-      </c>
       <c r="F22" t="n">
-        <v>126</v>
+        <v>464</v>
       </c>
     </row>
     <row r="23">
@@ -922,107 +922,107 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1240</v>
+        <v>1254</v>
       </c>
       <c r="C23" t="n">
-        <v>569</v>
+        <v>577</v>
       </c>
       <c r="D23" t="n">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E23" t="n">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F23" t="n">
-        <v>126</v>
+        <v>447</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>COLEGIO E CURSO MATRIZ EDUCACAO NOVA IGUACU</t>
+          <t>COLEGIO E CURSO MATRIZ EDUCACAO SÃO JOÃO DE MERITI</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1045</v>
+        <v>977</v>
       </c>
       <c r="C24" t="n">
-        <v>789</v>
+        <v>617</v>
       </c>
       <c r="D24" t="n">
-        <v>716</v>
+        <v>550</v>
       </c>
       <c r="E24" t="n">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="F24" t="n">
-        <v>120</v>
+        <v>446</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>COLEGIO SARAH DAWSEY - JUIZ DE FORA</t>
+          <t>COLÉGIOS INTEGRADOS LEONARDO DA VINCI - GAMA</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1143</v>
+        <v>815</v>
       </c>
       <c r="C25" t="n">
-        <v>445</v>
+        <v>369</v>
       </c>
       <c r="D25" t="n">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="E25" t="n">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="F25" t="n">
-        <v>119</v>
+        <v>443</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>COLÉGIO E CURSO MATRIZ EDUCACAO TIJUCA</t>
+          <t>COLÉGIO E CURSO AO CUBO BOTAFOGO</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1189</v>
+        <v>1212</v>
       </c>
       <c r="C26" t="n">
-        <v>607</v>
+        <v>386</v>
       </c>
       <c r="D26" t="n">
-        <v>527</v>
+        <v>232</v>
       </c>
       <c r="E26" t="n">
-        <v>120</v>
+        <v>164</v>
       </c>
       <c r="F26" t="n">
-        <v>119</v>
+        <v>366</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ESCOLA SA PEREIRA (R. DA MATRIZ)</t>
+          <t>COLEGIO E CURSO MATRIZ EDUCACAO DUQUE DE CAXIAS</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1086</v>
+        <v>918</v>
       </c>
       <c r="C27" t="n">
-        <v>451</v>
+        <v>674</v>
       </c>
       <c r="D27" t="n">
-        <v>269</v>
+        <v>618</v>
       </c>
       <c r="E27" t="n">
-        <v>163</v>
+        <v>287</v>
       </c>
       <c r="F27" t="n">
-        <v>107</v>
+        <v>347</v>
       </c>
     </row>
     <row r="28">
@@ -1032,370 +1032,282 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>859</v>
+        <v>866</v>
       </c>
       <c r="C28" t="n">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="D28" t="n">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E28" t="n">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="F28" t="n">
-        <v>101</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>COLÉGIOS INTEGRADOS LEONARDO DA VINCI - GAMA</t>
+          <t>COLEGIO E CURSO MATRIZ EDUCACAO NOVA IGUACU</t>
         </is>
       </c>
       <c r="B29" t="n">
+        <v>1069</v>
+      </c>
+      <c r="C29" t="n">
         <v>811</v>
       </c>
-      <c r="C29" t="n">
-        <v>368</v>
-      </c>
       <c r="D29" t="n">
-        <v>265</v>
+        <v>737</v>
       </c>
       <c r="E29" t="n">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="F29" t="n">
-        <v>98</v>
+        <v>321</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>COLÉGIO E CURSO AO CUBO BOTAFOGO</t>
+          <t>COLÉGIO QI FREGUESIA</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1206</v>
+        <v>800</v>
       </c>
       <c r="C30" t="n">
-        <v>383</v>
+        <v>216</v>
       </c>
       <c r="D30" t="n">
-        <v>231</v>
+        <v>126</v>
       </c>
       <c r="E30" t="n">
-        <v>164</v>
+        <v>105</v>
       </c>
       <c r="F30" t="n">
-        <v>96</v>
+        <v>321</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>COLÉGIO QI FREGUESIA</t>
+          <t>COLÉGIO QI VALQUEIRE</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>793</v>
+        <v>2693</v>
       </c>
       <c r="C31" t="n">
-        <v>215</v>
+        <v>765</v>
       </c>
       <c r="D31" t="n">
-        <v>127</v>
+        <v>610</v>
       </c>
       <c r="E31" t="n">
-        <v>104</v>
+        <v>563</v>
       </c>
       <c r="F31" t="n">
-        <v>82</v>
+        <v>292</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>COLÉGIO AMERICANO</t>
+          <t>CRECHE ESCOLA GLOBAL TREE - RIO 2</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>474</v>
+        <v>959</v>
       </c>
       <c r="C32" t="n">
-        <v>287</v>
+        <v>361</v>
       </c>
       <c r="D32" t="n">
-        <v>223</v>
+        <v>270</v>
       </c>
       <c r="E32" t="n">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="F32" t="n">
-        <v>71</v>
+        <v>248</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CRECHE ESCOLA GLOBAL TREE - ABM</t>
+          <t>COLEGIO E CURSO UNIAO LTDA</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>594</v>
+        <v>242</v>
       </c>
       <c r="C33" t="n">
-        <v>289</v>
+        <v>122</v>
       </c>
       <c r="D33" t="n">
-        <v>228</v>
+        <v>95</v>
       </c>
       <c r="E33" t="n">
-        <v>188</v>
+        <v>75</v>
       </c>
       <c r="F33" t="n">
-        <v>70</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CRECHE ESCOLA GLOBAL TREE - RECREIO</t>
+          <t>COLÉGIO E CURSO MATRIZ EDUCACAO TIJUCA</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1083</v>
+        <v>1208</v>
       </c>
       <c r="C34" t="n">
-        <v>389</v>
+        <v>625</v>
       </c>
       <c r="D34" t="n">
-        <v>232</v>
+        <v>544</v>
       </c>
       <c r="E34" t="n">
-        <v>187</v>
+        <v>120</v>
       </c>
       <c r="F34" t="n">
-        <v>69</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>INTEGRA EDUCACIONAL S/A</t>
+          <t>CRECHE ESCOLA GLOBAL TREE - PENINSULA</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>469</v>
+        <v>347</v>
       </c>
       <c r="C35" t="n">
-        <v>327</v>
+        <v>135</v>
       </c>
       <c r="D35" t="n">
-        <v>247</v>
+        <v>82</v>
       </c>
       <c r="E35" t="n">
-        <v>193</v>
+        <v>68</v>
       </c>
       <c r="F35" t="n">
-        <v>61</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CRECHE ESCOLA GLOBAL TREE - RIO 2</t>
+          <t>CRECHE ESCOLA GLOBAL TREE - ABM</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>952</v>
+        <v>598</v>
       </c>
       <c r="C36" t="n">
-        <v>357</v>
+        <v>290</v>
       </c>
       <c r="D36" t="n">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="E36" t="n">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F36" t="n">
-        <v>54</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CRECHE ESCOLA GLOBAL TREE - PENINSULA</t>
+          <t>CRECHE ESCOLA GLOBAL TREE - RECREIO</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>343</v>
+        <v>1090</v>
       </c>
       <c r="C37" t="n">
-        <v>135</v>
+        <v>397</v>
       </c>
       <c r="D37" t="n">
-        <v>82</v>
+        <v>237</v>
       </c>
       <c r="E37" t="n">
-        <v>68</v>
+        <v>187</v>
       </c>
       <c r="F37" t="n">
-        <v>34</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>BOM TEMPO CRECHE E EDUCACAO INFANTIL LTDA</t>
+          <t>APOGEU - PARÁ DE MINAS</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>609</v>
+        <v>1</v>
       </c>
       <c r="C38" t="n">
-        <v>245</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ESCOLA SÁ PEREIRA S.A. CAPISTRANO</t>
+          <t>COLÉGIO UNIFICADO INDEPENDÊNCIA</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>1126</v>
+        <v>1</v>
       </c>
       <c r="C39" t="n">
-        <v>429</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>258</v>
+        <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>COLEGIO E CURSO UNIAO LTDA</t>
+          <t>Leads Raiz Sem Unidades</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>238</v>
+        <v>4020</v>
       </c>
       <c r="C40" t="n">
-        <v>121</v>
+        <v>913</v>
       </c>
       <c r="D40" t="n">
-        <v>94</v>
+        <v>320</v>
       </c>
       <c r="E40" t="n">
-        <v>74</v>
+        <v>143</v>
       </c>
       <c r="F40" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>APOGEU - PARÁ DE MINAS</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>APOGEU - POUSO ALEGRE</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>4</v>
-      </c>
-      <c r="C42" t="n">
-        <v>1</v>
-      </c>
-      <c r="D42" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>COLÉGIO UNIFICADO INDEPENDÊNCIA</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>1</v>
-      </c>
-      <c r="C43" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Leads Raiz Sem Unidades</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>4009</v>
-      </c>
-      <c r="C44" t="n">
-        <v>911</v>
-      </c>
-      <c r="D44" t="n">
-        <v>320</v>
-      </c>
-      <c r="E44" t="n">
-        <v>143</v>
-      </c>
-      <c r="F44" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>